<commit_message>
Added lab 3exercises 1,4,5,6
</commit_message>
<xml_diff>
--- a/Teodora_Rabagel/Lab3.xlsx
+++ b/Teodora_Rabagel/Lab3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FacultateTeo\an 4\sem1\SOAC\Laborator\SOAC_23-24\Teodora_Rabagel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2001A8-09C4-4DC4-8D13-6AFBD823FD7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F571D5-6BA1-4117-83B2-D6661665DA86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1044" yWindow="1656" windowWidth="17280" windowHeight="8964" xr2:uid="{1C374C17-C950-4539-B60A-DEDCFF6C061C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1C374C17-C950-4539-B60A-DEDCFF6C061C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="33">
   <si>
     <t>Sort</t>
   </si>
@@ -121,6 +121,18 @@
   </si>
   <si>
     <t>DC_miss(BS=16, WB)</t>
+  </si>
+  <si>
+    <t>Aplicatia 6</t>
+  </si>
+  <si>
+    <t>IR(ideal)</t>
+  </si>
+  <si>
+    <t>IR(WB)</t>
+  </si>
+  <si>
+    <t>IR(wt)</t>
   </si>
 </sst>
 </file>
@@ -1806,6 +1818,2272 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Aplicatia 5 - IR</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CH"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IR(BS=4, WB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$54:$I$54</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$55:$I$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.94899999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6459999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.66900000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4830000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.47799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.67400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.30299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.53400000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EEDC-40CE-B96E-D67168971BBD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$56</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IR(BS=4, WT)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$54:$I$54</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$56:$I$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.80100000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.619</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.32300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.57399999999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.27900000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.39800000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EEDC-40CE-B96E-D67168971BBD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$57</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IR(BS=8, WB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$54:$I$54</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$57:$I$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0620000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.647</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.85799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4830000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.61899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.74199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.315</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.56899999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EEDC-40CE-B96E-D67168971BBD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$58</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IR(BS=8, WT)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$54:$I$54</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$58:$I$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.94499999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.633</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.59799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4810000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.46600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.65500000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.29899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.42299999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-EEDC-40CE-B96E-D67168971BBD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$59</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IR(BS=16, WB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$54:$I$54</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$59:$I$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.143</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.647</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0089999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4830000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.312</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.58299999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-EEDC-40CE-B96E-D67168971BBD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$60</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IR(BS=16, WT)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$54:$I$54</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$60:$I$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.056</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.46</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.753</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.482</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.58899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.72599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.29399999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.432</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-EEDC-40CE-B96E-D67168971BBD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="288597792"/>
+        <c:axId val="284597280"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="288597792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="284597280"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="284597280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="288597792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CH"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-CH"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Aplicatia 5 - DC_miss</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CH"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$63</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DC_miss(BS=4, WB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$62:$I$62</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$63:$I$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28.84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60.21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.93</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.54</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4205-4D75-B7EA-39CF0C836A23}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$64</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DC_miss(BS=4, WT)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$62:$I$62</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$64:$I$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28.84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60.21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.93</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.54</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4205-4D75-B7EA-39CF0C836A23}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$65</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DC_miss(BS=8, WB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$62:$I$62</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$65:$I$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>7.29</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.159999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.63</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30.14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4205-4D75-B7EA-39CF0C836A23}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DC_miss(BS=8, WT)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$62:$I$62</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$66:$I$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>7.29</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.159999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.63</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30.14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4205-4D75-B7EA-39CF0C836A23}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$67</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DC_miss(BS=16, WB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$62:$I$62</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$67:$I$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4.46</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.31</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.809999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.71</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.55</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28.36</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-4205-4D75-B7EA-39CF0C836A23}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$68</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DC_miss(BS=16, WT)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$62:$I$62</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$68:$I$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4.46</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.31</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.809999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.71</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.55</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28.36</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-4205-4D75-B7EA-39CF0C836A23}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="362697008"/>
+        <c:axId val="362696176"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="362697008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="362696176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="362696176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="362697008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CH"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-CH"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Aplicatia</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 6</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CH"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$85</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IR(ideal)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$84:$I$84</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$85:$I$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0580000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6479999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.70499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4830000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.505</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.81799999999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.308</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.65100000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E333-44AB-B9AE-F89F8368C3B8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IR(WB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$84:$I$84</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$86:$I$86</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.94899999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6459999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.66900000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4830000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.47799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.67400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.30299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.53400000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E333-44AB-B9AE-F89F8368C3B8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$87</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IR(wt)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$84:$I$84</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$87:$I$87</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.80100000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.619</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.32300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.57399999999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.27900000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.39800000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E333-44AB-B9AE-F89F8368C3B8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="288599872"/>
+        <c:axId val="288600288"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="288599872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="288600288"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="288600288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="288599872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CH"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-CH"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1926,6 +4204,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2933,6 +5331,1515 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3540,6 +7447,114 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A70AC21F-2B9C-4ACD-A5D7-21C2AA0FBCB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08C50429-8DF6-47BD-8EC9-38C3ED660630}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FA41CD0-FA3C-4F6A-B5A2-02B4D7AB218E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3845,10 +7860,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A69BE013-39F5-4977-908C-A77B9A8172A8}">
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="T89" sqref="T89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4277,26 +8292,146 @@
       <c r="A56" t="s">
         <v>18</v>
       </c>
+      <c r="B56">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="C56">
+        <v>1.619</v>
+      </c>
+      <c r="D56">
+        <v>0.43</v>
+      </c>
+      <c r="E56">
+        <v>1.48</v>
+      </c>
+      <c r="F56">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="G56">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="H56">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="I56">
+        <v>0.39800000000000002</v>
+      </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>19</v>
       </c>
+      <c r="B57">
+        <v>1.0620000000000001</v>
+      </c>
+      <c r="C57">
+        <v>1.647</v>
+      </c>
+      <c r="D57">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="E57">
+        <v>1.4830000000000001</v>
+      </c>
+      <c r="F57">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="G57">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="H57">
+        <v>0.315</v>
+      </c>
+      <c r="I57">
+        <v>0.56899999999999995</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>20</v>
       </c>
+      <c r="B58">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="C58">
+        <v>1.633</v>
+      </c>
+      <c r="D58">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="E58">
+        <v>1.4810000000000001</v>
+      </c>
+      <c r="F58">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="G58">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="H58">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="I58">
+        <v>0.42299999999999999</v>
+      </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>21</v>
       </c>
+      <c r="B59">
+        <v>1.143</v>
+      </c>
+      <c r="C59">
+        <v>1.647</v>
+      </c>
+      <c r="D59">
+        <v>1.0089999999999999</v>
+      </c>
+      <c r="E59">
+        <v>1.4830000000000001</v>
+      </c>
+      <c r="F59">
+        <v>0.72</v>
+      </c>
+      <c r="G59">
+        <v>0.8</v>
+      </c>
+      <c r="H59">
+        <v>0.312</v>
+      </c>
+      <c r="I59">
+        <v>0.58299999999999996</v>
+      </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>22</v>
       </c>
+      <c r="B60">
+        <v>1.056</v>
+      </c>
+      <c r="C60">
+        <v>1.46</v>
+      </c>
+      <c r="D60">
+        <v>0.753</v>
+      </c>
+      <c r="E60">
+        <v>1.482</v>
+      </c>
+      <c r="F60">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="G60">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="H60">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="I60">
+        <v>0.432</v>
+      </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
@@ -4329,53 +8464,291 @@
         <v>23</v>
       </c>
       <c r="B63">
-        <v>2064</v>
+        <v>12.1</v>
       </c>
       <c r="C63">
-        <v>218</v>
+        <v>0.36</v>
       </c>
       <c r="D63">
-        <v>19301</v>
+        <v>28.84</v>
       </c>
       <c r="E63">
-        <v>51</v>
+        <v>0.04</v>
       </c>
       <c r="F63">
-        <v>82433</v>
+        <v>60.21</v>
       </c>
       <c r="G63">
-        <v>10249</v>
+        <v>14.75</v>
       </c>
       <c r="H63">
-        <v>7647</v>
+        <v>7.93</v>
       </c>
       <c r="I63">
-        <v>12511</v>
+        <v>35.54</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>24</v>
       </c>
+      <c r="B64">
+        <v>12.1</v>
+      </c>
+      <c r="C64">
+        <v>0.36</v>
+      </c>
+      <c r="D64">
+        <v>28.84</v>
+      </c>
+      <c r="E64">
+        <v>0.04</v>
+      </c>
+      <c r="F64">
+        <v>60.21</v>
+      </c>
+      <c r="G64">
+        <v>14.75</v>
+      </c>
+      <c r="H64">
+        <v>7.93</v>
+      </c>
+      <c r="I64">
+        <v>35.54</v>
+      </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>25</v>
       </c>
+      <c r="B65">
+        <v>7.29</v>
+      </c>
+      <c r="C65">
+        <v>0.19</v>
+      </c>
+      <c r="D65">
+        <v>17.39</v>
+      </c>
+      <c r="E65">
+        <v>0.02</v>
+      </c>
+      <c r="F65">
+        <v>32.159999999999997</v>
+      </c>
+      <c r="G65">
+        <v>10.68</v>
+      </c>
+      <c r="H65">
+        <v>4.63</v>
+      </c>
+      <c r="I65">
+        <v>30.14</v>
+      </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>26</v>
       </c>
+      <c r="B66">
+        <v>7.29</v>
+      </c>
+      <c r="C66">
+        <v>0.19</v>
+      </c>
+      <c r="D66">
+        <v>17.39</v>
+      </c>
+      <c r="E66">
+        <v>0.02</v>
+      </c>
+      <c r="F66">
+        <v>32.159999999999997</v>
+      </c>
+      <c r="G66">
+        <v>10.68</v>
+      </c>
+      <c r="H66">
+        <v>4.63</v>
+      </c>
+      <c r="I66">
+        <v>30.14</v>
+      </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>28</v>
       </c>
+      <c r="B67">
+        <v>4.46</v>
+      </c>
+      <c r="C67">
+        <v>0.1</v>
+      </c>
+      <c r="D67">
+        <v>11.31</v>
+      </c>
+      <c r="E67">
+        <v>0.01</v>
+      </c>
+      <c r="F67">
+        <v>18.809999999999999</v>
+      </c>
+      <c r="G67">
+        <v>7.71</v>
+      </c>
+      <c r="H67">
+        <v>5.55</v>
+      </c>
+      <c r="I67">
+        <v>28.36</v>
+      </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>27</v>
+      </c>
+      <c r="B68">
+        <v>4.46</v>
+      </c>
+      <c r="C68">
+        <v>0.1</v>
+      </c>
+      <c r="D68">
+        <v>11.31</v>
+      </c>
+      <c r="E68">
+        <v>0.01</v>
+      </c>
+      <c r="F68">
+        <v>18.809999999999999</v>
+      </c>
+      <c r="G68">
+        <v>7.71</v>
+      </c>
+      <c r="H68">
+        <v>5.55</v>
+      </c>
+      <c r="I68">
+        <v>28.36</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
+        <v>0</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1</v>
+      </c>
+      <c r="D84" t="s">
+        <v>2</v>
+      </c>
+      <c r="E84" t="s">
+        <v>3</v>
+      </c>
+      <c r="F84" t="s">
+        <v>4</v>
+      </c>
+      <c r="G84" t="s">
+        <v>5</v>
+      </c>
+      <c r="H84" t="s">
+        <v>6</v>
+      </c>
+      <c r="I84" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>30</v>
+      </c>
+      <c r="B85">
+        <v>1.0580000000000001</v>
+      </c>
+      <c r="C85">
+        <v>1.6479999999999999</v>
+      </c>
+      <c r="D85">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="E85">
+        <v>1.4830000000000001</v>
+      </c>
+      <c r="F85">
+        <v>0.505</v>
+      </c>
+      <c r="G85">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="H85">
+        <v>0.308</v>
+      </c>
+      <c r="I85">
+        <v>0.65100000000000002</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>31</v>
+      </c>
+      <c r="B86">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="C86">
+        <v>1.6459999999999999</v>
+      </c>
+      <c r="D86">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="E86">
+        <v>1.4830000000000001</v>
+      </c>
+      <c r="F86">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="G86">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="H86">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="I86">
+        <v>0.53400000000000003</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>32</v>
+      </c>
+      <c r="B87">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="C87">
+        <v>1.619</v>
+      </c>
+      <c r="D87">
+        <v>0.43</v>
+      </c>
+      <c r="E87">
+        <v>1.48</v>
+      </c>
+      <c r="F87">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="G87">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="H87">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="I87">
+        <v>0.39800000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>